<commit_message>
propagating SingleLooseIsoEG/IsoEG approach to 0p9 and 0p6
</commit_message>
<xml_diff>
--- a/official/L1Menu_Collisions2022_v1_3_0/PrescaleTable/L1Menu_Collisions2022_v1_3_0-13.6TeV_2748b.xlsx
+++ b/official/L1Menu_Collisions2022_v1_3_0/PrescaleTable/L1Menu_Collisions2022_v1_3_0-13.6TeV_2748b.xlsx
@@ -1368,16 +1368,16 @@
     <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="0" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="3" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
@@ -1549,9 +1549,9 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
               <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
+                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -1631,7 +1631,7 @@
         </a:effectLst>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -1659,10 +1659,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -1918,9 +1918,9 @@
           <a:round/>
         </a:ln>
         <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="20000" dir="5400000">
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="23000" dir="5400000">
             <a:srgbClr val="000000">
-              <a:alpha val="38000"/>
+              <a:alpha val="35000"/>
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
@@ -2208,7 +2208,7 @@
         <a:effectLst/>
         <a:sp3d/>
       </a:spPr>
-      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45719" tIns="45719" rIns="45719" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
+      <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="45718" tIns="45718" rIns="45718" bIns="45718" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
@@ -2236,10 +2236,10 @@
             </a:solidFill>
             <a:effectLst/>
             <a:uFillTx/>
-            <a:latin typeface="Calibri"/>
-            <a:ea typeface="Calibri"/>
-            <a:cs typeface="Calibri"/>
-            <a:sym typeface="Calibri"/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -2497,7 +2497,7 @@
   <sheetFormatPr defaultColWidth="8.83333" defaultRowHeight="15" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col min="1" max="1" width="8.85156" style="1" customWidth="1"/>
-    <col min="2" max="2" width="48.0312" style="1" customWidth="1"/>
+    <col min="2" max="2" width="48" style="1" customWidth="1"/>
     <col min="3" max="11" width="8.85156" style="1" customWidth="1"/>
     <col min="12" max="256" width="8.85156" style="1" customWidth="1"/>
   </cols>
@@ -7956,10 +7956,10 @@
         <v>0</v>
       </c>
       <c r="J156" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K156" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="157" ht="15" customHeight="1">
@@ -8026,10 +8026,10 @@
         <v>0</v>
       </c>
       <c r="J158" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K158" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="159" ht="15" customHeight="1">
@@ -8061,10 +8061,10 @@
         <v>0</v>
       </c>
       <c r="J159" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K159" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="160" ht="15" customHeight="1">
@@ -8131,10 +8131,10 @@
         <v>0</v>
       </c>
       <c r="J161" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K161" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="162" ht="15" customHeight="1">
@@ -8411,10 +8411,10 @@
         <v>0</v>
       </c>
       <c r="J169" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K169" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="170" ht="15" customHeight="1">
@@ -8446,10 +8446,10 @@
         <v>0</v>
       </c>
       <c r="J170" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K170" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="171" ht="15" customHeight="1">
@@ -10161,10 +10161,10 @@
         <v>0</v>
       </c>
       <c r="J219" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K219" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="220" ht="15" customHeight="1">
@@ -12348,28 +12348,28 @@
         <v>0</v>
       </c>
       <c r="D282" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E282" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F282" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G282" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H282" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I282" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J282" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K282" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="283" ht="15" customHeight="1">
@@ -12383,28 +12383,28 @@
         <v>0</v>
       </c>
       <c r="D283" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E283" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F283" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G283" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H283" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I283" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J283" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K283" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="284" ht="15" customHeight="1">

</xml_diff>